<commit_message>
Revisi Indeks Pendidikan & Indeks Pengeluaran Banyuwangi
</commit_message>
<xml_diff>
--- a/Rekap/RekapDimensiPengeluaran.xlsx
+++ b/Rekap/RekapDimensiPengeluaran.xlsx
@@ -115,10 +115,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="&quot;Rp&quot;#,##0"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -161,30 +161,67 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -192,38 +229,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -237,16 +251,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -260,45 +274,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -313,175 +313,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,39 +532,6 @@
         <color auto="1"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -607,6 +574,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -624,157 +602,179 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1138,7 +1138,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1386,7 +1386,7 @@
         <v>10742914</v>
       </c>
       <c r="D17" s="6">
-        <v>0.71</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="18" ht="15.75" spans="1:4">

</xml_diff>

<commit_message>
Revisi Indeks Pengeluaran Wongsorejo
</commit_message>
<xml_diff>
--- a/Rekap/RekapDimensiPengeluaran.xlsx
+++ b/Rekap/RekapDimensiPengeluaran.xlsx
@@ -114,11 +114,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="&quot;Rp&quot;#,##0"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="&quot;Rp&quot;#,##0"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -161,12 +161,27 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -175,16 +190,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -192,21 +207,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -221,15 +230,43 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -251,21 +288,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -274,31 +296,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -313,25 +313,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -343,157 +481,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,6 +532,26 @@
         <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -574,13 +594,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -599,182 +632,149 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -792,7 +792,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -801,7 +801,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -813,7 +813,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1138,7 +1138,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1414,7 +1414,7 @@
         <v>9972669</v>
       </c>
       <c r="D19" s="6">
-        <v>0.73</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="20" ht="15.75" spans="1:4">

</xml_diff>